<commit_message>
gradient boosting regression update
</commit_message>
<xml_diff>
--- a/code/predictive modeling/funkcni/funcni data set - Copy.xlsx
+++ b/code/predictive modeling/funkcni/funcni data set - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f619c9dbaff66258/development/github/sws/code/predictive modeling/funkcni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{7CD2E4E8-1F28-44FE-ADE5-F3B50EE5FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22ACFD7E-32FF-4F71-9A1B-B1F98DC4054C}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{7CD2E4E8-1F28-44FE-ADE5-F3B50EE5FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5987EAAB-7B69-4E54-93B1-88B18A4D32C6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DC190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q64" workbookViewId="0">
-      <selection activeCell="AQ103" sqref="AQ103"/>
+    <sheetView tabSelected="1" topLeftCell="AE89" workbookViewId="0">
+      <selection activeCell="AR107" sqref="AR107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>